<commit_message>
Client: Add MoveState Stamina Cotrol System
스테미나가 없으면 달리지 못하게 수정
</commit_message>
<xml_diff>
--- a/Client/Assets/11. GameData/Ch_Stat.xlsx
+++ b/Client/Assets/11. GameData/Ch_Stat.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\FestivalTownProject\Client\Assets\11. GameData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADD313A1-0D04-435B-BE4A-CB4A2244B33A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25605" yWindow="3165" windowWidth="22680" windowHeight="11295" xr2:uid="{6B7BBA14-F215-42A1-AF74-6DAD170DC25E}"/>
+    <workbookView xWindow="-25605" yWindow="3165" windowWidth="22680" windowHeight="11295" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Stat" sheetId="2" r:id="rId1"/>
-    <sheet name="Attack" sheetId="1" r:id="rId2"/>
-    <sheet name="Move" sheetId="3" r:id="rId3"/>
-    <sheet name="Action" sheetId="5" r:id="rId4"/>
+    <sheet name="Stat" sheetId="2" r:id="rId4"/>
+    <sheet name="Attack" sheetId="1" r:id="rId5"/>
+    <sheet name="Move" sheetId="3" r:id="rId6"/>
+    <sheet name="Action" sheetId="5" r:id="rId7"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,83 +38,96 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>tc={7CAEFB94-C44A-4722-A60F-00FE1A6A230F}</author>
-    <author>tc={95A83C7F-F844-44CE-9E40-79C2287106B4}</author>
-    <author>tc={CA403F8E-AE87-4D0C-A052-22EB6FF64D5A}</author>
-    <author>tc={C076C02E-2F86-45E9-9272-E00A80B69A6C}</author>
-    <author>tc={F07E6F01-F6BB-4234-B0DD-E67FD4058A27}</author>
-  </authors>
-  <commentList>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{7CAEFB94-C44A-4722-A60F-00FE1A6A230F}">
-      <text>
-        <t>[스레드 댓글]
-사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
-댓글:
-    Value = 0 -&gt;  해당사항없음</t>
-      </text>
-    </comment>
-    <comment ref="D1" authorId="1" shapeId="0" xr:uid="{95A83C7F-F844-44CE-9E40-79C2287106B4}">
-      <text>
-        <t>[스레드 댓글]
-사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
-댓글:
-    공격속도</t>
-      </text>
-    </comment>
-    <comment ref="E1" authorId="2" shapeId="0" xr:uid="{CA403F8E-AE87-4D0C-A052-22EB6FF64D5A}">
-      <text>
-        <t>[스레드 댓글]
-사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
-댓글:
-    M로 계산</t>
-      </text>
-    </comment>
-    <comment ref="F1" authorId="3" shapeId="0" xr:uid="{C076C02E-2F86-45E9-9272-E00A80B69A6C}">
-      <text>
-        <t>[스레드 댓글]
-사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
-댓글:
-    스테미나 소모값
-Ch_Hold는 초당으로 계산</t>
-      </text>
-    </comment>
-    <comment ref="G1" authorId="4" shapeId="0" xr:uid="{F07E6F01-F6BB-4234-B0DD-E67FD4058A27}">
-      <text>
-        <t>[스레드 댓글]
-사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
-댓글:
-    공격 성공 시 상대방이 깍이는 스테미나</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={ED658604-CAEF-454D-8323-3066716088AE}</author>
-    <author>tc={2AA21D1F-7D2F-426A-B782-8B6AB840ED89}</author>
+    <author>김혁동(2017180008)</author>
   </authors>
   <commentList>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{ED658604-CAEF-454D-8323-3066716088AE}">
+    <comment ref="C1" authorId="0">
       <text>
-        <t>[스레드 댓글]
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>[스레드 댓글]
 사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
 댓글:
-    Value = 0 이면 해당사항 없음</t>
+  Value = 0 -&gt;  해당사항없음</t>
+        </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="1" shapeId="0" xr:uid="{2AA21D1F-7D2F-426A-B782-8B6AB840ED89}">
+    <comment ref="D1" authorId="0">
       <text>
-        <t>[스레드 댓글]
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>[스레드 댓글]
 사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
 댓글:
-    초당으로 계산
-Ch_Dash는 횟수로 계산</t>
+  공격속도</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>[스레드 댓글]
+사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
+댓글:
+  M로 계산</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>[스레드 댓글]
+사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
+댓글:
+  스테미나 소모값
+Ch_Hold는 초당으로 계산</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>[스레드 댓글]
+사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
+댓글:
+  공격 성공 시 상대방이 깍이는 스테미나</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -124,37 +137,107 @@
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={8EA9EDC3-CDA5-4BC8-B6E1-AC66720DED88}</author>
-    <author>tc={9E67C2FE-2272-4746-AF93-2ADEBE077AFF}</author>
-    <author>tc={04AB212E-1ECE-4681-84F1-FB2C04EC020A}</author>
+    <author>김혁동(2017180008)</author>
   </authors>
   <commentList>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{8EA9EDC3-CDA5-4BC8-B6E1-AC66720DED88}">
+    <comment ref="C1" authorId="0">
       <text>
-        <t>[스레드 댓글]
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>[스레드 댓글]
 사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
 댓글:
-    행동속도 (초로 계산)</t>
+  Value = 0 이면 해당사항 없음</t>
+        </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="1" shapeId="0" xr:uid="{9E67C2FE-2272-4746-AF93-2ADEBE077AFF}">
+    <comment ref="D1" authorId="0">
       <text>
-        <t>[스레드 댓글]
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>[스레드 댓글]
 사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
 댓글:
-    오브젝트와 거리 
+  초당으로 계산
+Ch_Dash는 횟수로 계산</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>김혁동(2017180008)</author>
+  </authors>
+  <commentList>
+    <comment ref="C1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>[스레드 댓글]
+사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
+댓글:
+  행동속도 (초로 계산)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>[스레드 댓글]
+사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
+댓글:
+  오브젝트와 거리 
 원 모양
 반지름으로 계산
 M로 계산</t>
+        </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="2" shapeId="0" xr:uid="{04AB212E-1ECE-4681-84F1-FB2C04EC020A}">
+    <comment ref="E1" authorId="0">
       <text>
-        <t>[스레드 댓글]
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>[스레드 댓글]
 사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
 댓글:
-    스테미나 소모값
+  스테미나 소모값
 Ch_Hold는 초당으로 계산</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -165,137 +248,106 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
   <si>
     <t>Ch_Attack</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Ch_HeadAttack</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Ch_JumpAttack</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Ch_PowerAttack</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Ch_Hold</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Attack_Speed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Ch_StaminaConsume</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Ch_Hp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Ch_Stamina</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Ch_Speed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Cat</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Index</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Ch_Walk</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Ch_Run</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Ch_Dash</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Value</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Ch_Strength</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Ch_Jump</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Ch_Stamina_recovery</t>
   </si>
   <si>
     <t>Ch_Idle</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Ch_Throw</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Ch_HoldWalk</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Ch_HoldRun</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Attack_Range</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Ch_WeaponPick</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Ch_BombPick</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Action_Speed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Action_Range</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Vanish_Stamina</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Ch_HoldJump</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Ch_WeaponAttack</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -303,6 +355,12 @@
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -344,27 +402,119 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
+      <protection/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="15" builtinId="5"/>
+    <cellStyle name="Currency" xfId="16" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="17" builtinId="7"/>
+    <cellStyle name="Comma" xfId="18" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="19" builtinId="6"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -697,66 +847,15 @@
 </a:theme>
 </file>
 
-<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="C1" dT="2024-09-27T13:44:35.54" personId="{9097131C-C7F7-4B7C-95CC-7296F4277D5E}" id="{7CAEFB94-C44A-4722-A60F-00FE1A6A230F}">
-    <text>Value = 0 -&gt;  해당사항없음</text>
-  </threadedComment>
-  <threadedComment ref="D1" dT="2024-09-27T14:20:20.98" personId="{9097131C-C7F7-4B7C-95CC-7296F4277D5E}" id="{95A83C7F-F844-44CE-9E40-79C2287106B4}">
-    <text>공격속도</text>
-  </threadedComment>
-  <threadedComment ref="E1" dT="2024-10-01T07:00:48.84" personId="{9097131C-C7F7-4B7C-95CC-7296F4277D5E}" id="{CA403F8E-AE87-4D0C-A052-22EB6FF64D5A}">
-    <text>M로 계산</text>
-  </threadedComment>
-  <threadedComment ref="F1" dT="2024-09-27T13:45:13.24" personId="{9097131C-C7F7-4B7C-95CC-7296F4277D5E}" id="{C076C02E-2F86-45E9-9272-E00A80B69A6C}">
-    <text>스테미나 소모값
-Ch_Hold는 초당으로 계산</text>
-  </threadedComment>
-  <threadedComment ref="G1" dT="2024-09-27T14:21:22.69" personId="{9097131C-C7F7-4B7C-95CC-7296F4277D5E}" id="{F07E6F01-F6BB-4234-B0DD-E67FD4058A27}">
-    <text>공격 성공 시 상대방이 깍이는 스테미나</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
-<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="C1" dT="2024-09-27T14:14:02.45" personId="{9097131C-C7F7-4B7C-95CC-7296F4277D5E}" id="{ED658604-CAEF-454D-8323-3066716088AE}">
-    <text>Value = 0 이면 해당사항 없음</text>
-  </threadedComment>
-  <threadedComment ref="D1" dT="2024-09-27T13:45:13.24" personId="{9097131C-C7F7-4B7C-95CC-7296F4277D5E}" id="{2AA21D1F-7D2F-426A-B782-8B6AB840ED89}">
-    <text>초당으로 계산
-Ch_Dash는 횟수로 계산</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
-<file path=xl/threadedComments/threadedComment3.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="C1" dT="2024-09-27T14:20:20.98" personId="{9097131C-C7F7-4B7C-95CC-7296F4277D5E}" id="{8EA9EDC3-CDA5-4BC8-B6E1-AC66720DED88}">
-    <text>행동속도 (초로 계산)</text>
-  </threadedComment>
-  <threadedComment ref="D1" dT="2024-10-01T07:00:48.84" personId="{9097131C-C7F7-4B7C-95CC-7296F4277D5E}" id="{9E67C2FE-2272-4746-AF93-2ADEBE077AFF}">
-    <text>오브젝트와 거리 
-원 모양
-반지름으로 계산
-M로 계산</text>
-  </threadedComment>
-  <threadedComment ref="E1" dT="2024-09-27T13:45:13.24" personId="{9097131C-C7F7-4B7C-95CC-7296F4277D5E}" id="{04AB212E-1ECE-4681-84F1-FB2C04EC020A}">
-    <text>스테미나 소모값
-Ch_Hold는 초당으로 계산</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F961BFE-AEF0-4053-AE30-EADB432CB913}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F961BFE-AEF0-4053-AE30-EADB432CB913}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0" topLeftCell="A1">
+      <selection pane="topLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.25" bestFit="1" customWidth="1"/>
@@ -768,7 +867,7 @@
     <col min="10" max="12" width="9.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="20.25">
       <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
@@ -788,7 +887,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="16.5">
       <c r="A2">
         <v>1000</v>
       </c>
@@ -809,20 +908,19 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AB07990-B5DE-4DA3-A25A-FCE377F249C7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AB07990-B5DE-4DA3-A25A-FCE377F249C7}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0" topLeftCell="A1">
+      <selection pane="topLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="7.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.875" bestFit="1" customWidth="1"/>
@@ -833,7 +931,7 @@
     <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="20.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -856,7 +954,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="16.5">
       <c r="A2">
         <v>10001</v>
       </c>
@@ -864,7 +962,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0.5</v>
+        <v>0.50</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -879,7 +977,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="16.5">
       <c r="A3">
         <v>10002</v>
       </c>
@@ -887,13 +985,13 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>1.3</v>
+        <v>1.30</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3">
-        <v>1.3</v>
+        <v>1.30</v>
       </c>
       <c r="F3">
         <v>10</v>
@@ -902,7 +1000,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="16.5">
       <c r="A4">
         <v>10003</v>
       </c>
@@ -916,7 +1014,7 @@
         <v>1</v>
       </c>
       <c r="E4">
-        <v>1.4</v>
+        <v>1.40</v>
       </c>
       <c r="F4">
         <v>15</v>
@@ -925,7 +1023,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="16.5">
       <c r="A5">
         <v>10004</v>
       </c>
@@ -948,7 +1046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="16.5">
       <c r="A6">
         <v>10005</v>
       </c>
@@ -971,7 +1069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="16.5">
       <c r="A7">
         <v>10006</v>
       </c>
@@ -979,13 +1077,13 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>0.8</v>
+        <v>0.80</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7">
-        <v>0.3</v>
+        <v>0.30</v>
       </c>
       <c r="F7">
         <v>8</v>
@@ -994,7 +1092,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="16.5">
       <c r="A8">
         <v>10007</v>
       </c>
@@ -1018,21 +1116,20 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C159E774-2D2E-4E42-A34F-C2E138094600}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C159E774-2D2E-4E42-A34F-C2E138094600}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1">
+      <selection pane="topLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.375" bestFit="1" customWidth="1"/>
@@ -1041,7 +1138,7 @@
     <col min="5" max="5" width="26.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="20.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -1058,7 +1155,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="16.5">
       <c r="A2">
         <v>20001</v>
       </c>
@@ -1075,7 +1172,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="16.5">
       <c r="A3">
         <v>20002</v>
       </c>
@@ -1083,7 +1180,7 @@
         <v>12</v>
       </c>
       <c r="C3">
-        <v>0.2</v>
+        <v>0.50</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -1092,7 +1189,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="16.5">
       <c r="A4">
         <v>20003</v>
       </c>
@@ -1100,7 +1197,7 @@
         <v>13</v>
       </c>
       <c r="C4">
-        <v>0.4</v>
+        <v>0.80</v>
       </c>
       <c r="D4">
         <v>5</v>
@@ -1109,7 +1206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="16.5">
       <c r="A5">
         <v>20004</v>
       </c>
@@ -1126,7 +1223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="16.5">
       <c r="A6">
         <v>20005</v>
       </c>
@@ -1134,7 +1231,7 @@
         <v>14</v>
       </c>
       <c r="C6">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="D6">
         <v>10</v>
@@ -1143,7 +1240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="16.5">
       <c r="A7">
         <v>20006</v>
       </c>
@@ -1151,7 +1248,7 @@
         <v>21</v>
       </c>
       <c r="C7">
-        <v>0.17</v>
+        <v>0.40</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -1160,7 +1257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="16.5">
       <c r="A8">
         <v>20007</v>
       </c>
@@ -1168,7 +1265,7 @@
         <v>22</v>
       </c>
       <c r="C8">
-        <v>0.3</v>
+        <v>0.70</v>
       </c>
       <c r="D8">
         <v>5</v>
@@ -1177,7 +1274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="16.5">
       <c r="A9">
         <v>20008</v>
       </c>
@@ -1195,21 +1292,20 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E578D4C-D8A7-4CED-8428-0F9C08F4A41C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E578D4C-D8A7-4CED-8428-0F9C08F4A41C}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0" topLeftCell="A1">
+      <selection pane="topLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="2" max="2" width="15.25" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
@@ -1217,7 +1313,7 @@
     <col min="5" max="5" width="27.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="20.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -1234,7 +1330,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="16.5">
       <c r="A2">
         <v>30001</v>
       </c>
@@ -1242,7 +1338,7 @@
         <v>24</v>
       </c>
       <c r="C2">
-        <v>0.5</v>
+        <v>0.50</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1251,7 +1347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="16.5">
       <c r="A3">
         <v>30002</v>
       </c>
@@ -1259,7 +1355,7 @@
         <v>25</v>
       </c>
       <c r="C3">
-        <v>0.5</v>
+        <v>0.50</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1269,8 +1365,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>